<commit_message>
Back into it! Big changes, via SQL
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\NBR\20. NBR\780 5T Growth model\780_growth_model\clone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\NBR\20. NBR\905 Nordic Beet Yield Challenge NBYC\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -253,7 +253,7 @@
     <t>Windspeed</t>
   </si>
   <si>
-    <t>RUEZero</t>
+    <t>rue_zero</t>
   </si>
 </sst>
 </file>

</xml_diff>